<commit_message>
Models validation during different months of 2018
</commit_message>
<xml_diff>
--- a/April 2018/Saturday_Sunday_Weekday/Validation/Input_April2018.xlsx
+++ b/April 2018/Saturday_Sunday_Weekday/Validation/Input_April2018.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20372"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B833E54-97C4-4BED-B5F1-58255341A6F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23437F41-803B-4127-A912-7ABA05D48E1F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1246,7 +1246,7 @@
   <dimension ref="E4:U33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>